<commit_message>
Add validation ("test") to Data.xlsx, auto_mlr
Add optional validation data, including pred_vs_act plotting
</commit_message>
<xml_diff>
--- a/src/Data.xlsx
+++ b/src/Data.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marc\Atmonia Dropbox\Marc Francis Hidalgo\Scripts\How to DoE and ML\ML\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3455ED19-1BD0-4F65-9E34-248DD2ECEDE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{505E8CA6-B55A-49D3-AB48-BE9F514299AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{C1646789-F2F7-4596-96D5-A1743CEE8B52}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{C1646789-F2F7-4596-96D5-A1743CEE8B52}"/>
   </bookViews>
   <sheets>
-    <sheet name="Data" sheetId="2" r:id="rId1"/>
-    <sheet name="Design Parameters" sheetId="1" r:id="rId2"/>
-    <sheet name="Responses" sheetId="3" r:id="rId3"/>
+    <sheet name="Train Data" sheetId="4" r:id="rId1"/>
+    <sheet name="Test Data" sheetId="2" r:id="rId2"/>
+    <sheet name="Design Parameters" sheetId="1" r:id="rId3"/>
+    <sheet name="Responses" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,6 +41,24 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>tc={AF751126-B492-47A8-A21F-68667097EBC7}</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{AF751126-B492-47A8-A21F-68667097EBC7}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Column names should be names for the features or responses. The subsequent rows should contain the actual data. Each row should basically be a single experiment. Add as many rows and columns as needed. </t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
     <author>tc={B4CB8F19-F74F-49D3-B51E-B8AFA5AE1E35}</author>
   </authors>
   <commentList>
@@ -55,7 +74,7 @@
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={A129F280-6E28-46E6-B655-4ABBE0C15904}</author>
@@ -109,7 +128,7 @@
 </comments>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={63297DB1-226E-491F-970B-DCA494C9496F}</author>
@@ -143,7 +162,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
   <si>
     <t>Features</t>
   </si>
@@ -164,13 +183,31 @@
   </si>
   <si>
     <t>Term type</t>
+  </si>
+  <si>
+    <t>Run</t>
+  </si>
+  <si>
+    <t>Roll temperature (°C)</t>
+  </si>
+  <si>
+    <t>Target density (g/cm3)</t>
+  </si>
+  <si>
+    <t>Calculated target porosity (%)</t>
+  </si>
+  <si>
+    <t>C/5-6 (mAh/g)</t>
+  </si>
+  <si>
+    <t>10C (mAh/g)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -184,12 +221,6 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -575,13 +606,21 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A1" dT="2024-07-09T18:28:17.65" personId="{1DB282FF-D362-47DF-A85A-03995C31D022}" id="{AF751126-B492-47A8-A21F-68667097EBC7}">
+    <text xml:space="preserve">Column names should be names for the features or responses. The subsequent rows should contain the actual data. Each row should basically be a single experiment. Add as many rows and columns as needed. </text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <threadedComment ref="A1" dT="2024-07-09T18:28:17.65" personId="{1DB282FF-D362-47DF-A85A-03995C31D022}" id="{B4CB8F19-F74F-49D3-B51E-B8AFA5AE1E35}">
     <text xml:space="preserve">Column names should be names for the features or responses. The subsequent rows should contain the actual data. Each row should basically be a single experiment. Add as many rows and columns as needed. </text>
   </threadedComment>
 </ThreadedComments>
 </file>
 
-<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/threadedComments/threadedComment3.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <threadedComment ref="A1" dT="2024-06-17T20:07:14.73" personId="{1DB282FF-D362-47DF-A85A-03995C31D022}" id="{A129F280-6E28-46E6-B655-4ABBE0C15904}">
     <text>Should be single letters and CANNOT BE C (i.e. A, B, D, etc.)</text>
@@ -601,7 +640,7 @@
 </ThreadedComments>
 </file>
 
-<file path=xl/threadedComments/threadedComment3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/threadedComments/threadedComment4.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <threadedComment ref="A1" dT="2024-07-09T18:33:32.98" personId="{1DB282FF-D362-47DF-A85A-03995C31D022}" id="{63297DB1-226E-491F-970B-DCA494C9496F}">
     <text>Name of each response. Should match the names in the “Data” sheet</text>
@@ -619,22 +658,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C2412BF-878C-45DB-8461-781C8212B1FA}">
-  <dimension ref="A1:F19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7017105-9951-4AAA-B498-721790E5798E}">
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A17" sqref="A2:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="2"/>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+    <row r="1" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="7"/>
@@ -726,24 +777,6 @@
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -752,11 +785,66 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C2412BF-878C-45DB-8461-781C8212B1FA}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1A90CAD-67BE-406A-8BD7-81EDC587CCAA}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -805,12 +893,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43A8F6C1-4570-407C-96BE-50A819E04C7D}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Add categorical functionality for MLR
Works as intended so far. Known bug where AICc does not match AICc from DesignExpert, but BIC works fine.
Needs testing before can be pushed to main.
</commit_message>
<xml_diff>
--- a/src/Data.xlsx
+++ b/src/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marc\Atmonia Dropbox\Marc Francis Hidalgo\Scripts\How to DoE and ML\ML\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89758752-27F4-4DBE-9743-A9B4398000B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{702F871E-A47D-4034-AD3D-7D4D9097CB6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C1646789-F2F7-4596-96D5-A1743CEE8B52}"/>
   </bookViews>
@@ -100,28 +100,31 @@
     Each row is the name of each feature. Should match the feature names in the “Data” sheet </t>
       </text>
     </comment>
-    <comment ref="C1" authorId="2" shapeId="0" xr:uid="{53826AD9-B736-4EE5-941D-FCB297D9709B}">
+    <comment ref="D1" authorId="2" shapeId="0" xr:uid="{53826AD9-B736-4EE5-941D-FCB297D9709B}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    The minimum level of this feature.</t>
+    The minimum level of this feature.
+Only applicable to numerical features, will be ignored if feature is categorical,</t>
       </text>
     </comment>
-    <comment ref="D1" authorId="3" shapeId="0" xr:uid="{BACBF89F-6AA0-4BCD-901B-3E077AF7EA4A}">
+    <comment ref="E1" authorId="3" shapeId="0" xr:uid="{BACBF89F-6AA0-4BCD-901B-3E077AF7EA4A}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    The maximum level of this feature.</t>
+    The maximum level of this feature.
+Only applicable to numerical features, will be ignored if feature is categorical,</t>
       </text>
     </comment>
-    <comment ref="E1" authorId="4" shapeId="0" xr:uid="{BA8E9C76-46BD-44C8-981A-1CC2357C5CAF}">
+    <comment ref="F1" authorId="4" shapeId="0" xr:uid="{BA8E9C76-46BD-44C8-981A-1CC2357C5CAF}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Dropdown, denotes whether the feature is a Mixture or Process feature. When in doubt, set to Process.</t>
+    Dropdown, denotes whether the feature is a Mixture or Process feature. When in doubt, set to Process.
+Only applicable to numerical features, will be ignored if feature is categorical,</t>
       </text>
     </comment>
   </commentList>
@@ -162,7 +165,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="25">
   <si>
     <t>Features</t>
   </si>
@@ -183,6 +186,60 @@
   </si>
   <si>
     <t>Term type</t>
+  </si>
+  <si>
+    <t>Run</t>
+  </si>
+  <si>
+    <t>Roll temperature (°C)</t>
+  </si>
+  <si>
+    <t>Target density (g/cm3)</t>
+  </si>
+  <si>
+    <t>Calculated target porosity (%)</t>
+  </si>
+  <si>
+    <t>C/5-6 (mAh/g)</t>
+  </si>
+  <si>
+    <t>10C (mAh/g)</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Process</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>-1,0,1</t>
+  </si>
+  <si>
+    <t>-1, 0, 1</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>mid</t>
+  </si>
+  <si>
+    <t>Feature type</t>
+  </si>
+  <si>
+    <t>Numerical</t>
+  </si>
+  <si>
+    <t>Categorical</t>
   </si>
 </sst>
 </file>
@@ -225,7 +282,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -246,6 +303,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -610,14 +670,17 @@
   <threadedComment ref="B1" dT="2024-07-09T18:31:44.34" personId="{1DB282FF-D362-47DF-A85A-03995C31D022}" id="{BC7AD3A8-5E18-4A5C-9728-B3CD7668C3E2}">
     <text xml:space="preserve">Each row is the name of each feature. Should match the feature names in the “Data” sheet </text>
   </threadedComment>
-  <threadedComment ref="C1" dT="2024-07-09T18:32:18.60" personId="{1DB282FF-D362-47DF-A85A-03995C31D022}" id="{53826AD9-B736-4EE5-941D-FCB297D9709B}">
-    <text>The minimum level of this feature.</text>
+  <threadedComment ref="D1" dT="2024-07-09T18:32:18.60" personId="{1DB282FF-D362-47DF-A85A-03995C31D022}" id="{53826AD9-B736-4EE5-941D-FCB297D9709B}">
+    <text>The minimum level of this feature.
+Only applicable to numerical features, will be ignored if feature is categorical,</text>
   </threadedComment>
-  <threadedComment ref="D1" dT="2024-07-09T18:32:26.48" personId="{1DB282FF-D362-47DF-A85A-03995C31D022}" id="{BACBF89F-6AA0-4BCD-901B-3E077AF7EA4A}">
-    <text>The maximum level of this feature.</text>
+  <threadedComment ref="E1" dT="2024-07-09T18:32:26.48" personId="{1DB282FF-D362-47DF-A85A-03995C31D022}" id="{BACBF89F-6AA0-4BCD-901B-3E077AF7EA4A}">
+    <text>The maximum level of this feature.
+Only applicable to numerical features, will be ignored if feature is categorical,</text>
   </threadedComment>
-  <threadedComment ref="E1" dT="2024-07-09T18:33:05.39" personId="{1DB282FF-D362-47DF-A85A-03995C31D022}" id="{BA8E9C76-46BD-44C8-981A-1CC2357C5CAF}">
-    <text>Dropdown, denotes whether the feature is a Mixture or Process feature. When in doubt, set to Process.</text>
+  <threadedComment ref="F1" dT="2024-07-09T18:33:05.39" personId="{1DB282FF-D362-47DF-A85A-03995C31D022}" id="{BA8E9C76-46BD-44C8-981A-1CC2357C5CAF}">
+    <text>Dropdown, denotes whether the feature is a Mixture or Process feature. When in doubt, set to Process.
+Only applicable to numerical features, will be ignored if feature is categorical,</text>
   </threadedComment>
 </ThreadedComments>
 </file>
@@ -643,126 +706,348 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7017105-9951-4AAA-B498-721790E5798E}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="2"/>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+    <row r="1" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7">
+        <v>85</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2">
+        <v>161.26647034381304</v>
+      </c>
+      <c r="F2">
+        <v>72.041289257868158</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
+      <c r="A3" s="7">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7">
+        <v>85</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3">
+        <v>163.24631274749157</v>
+      </c>
+      <c r="F3">
+        <v>85.186684022091868</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
+      <c r="A4" s="7">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7">
+        <v>85</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4">
+        <v>163.61126514902989</v>
+      </c>
+      <c r="F4">
+        <v>89.828855429747492</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
+      <c r="A5" s="7">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7">
+        <v>120</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5">
+        <v>162.54669346536949</v>
+      </c>
+      <c r="F5">
+        <v>59.174622450856383</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
+      <c r="A6" s="7">
+        <v>6</v>
+      </c>
+      <c r="B6" s="7">
+        <v>120</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6">
+        <v>162.57257207035542</v>
+      </c>
+      <c r="F6">
+        <v>84.951190961672879</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
+      <c r="A7" s="7">
+        <v>7</v>
+      </c>
+      <c r="B7" s="7">
+        <v>145</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7">
+        <v>160.60330891119415</v>
+      </c>
+      <c r="F7">
+        <v>30.733031121982521</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
+      <c r="A8" s="7">
+        <v>8</v>
+      </c>
+      <c r="B8" s="7">
+        <v>145</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8">
+        <v>161.72268604850387</v>
+      </c>
+      <c r="F8">
+        <v>84.945758440531378</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
+      <c r="A9" s="7">
+        <v>9</v>
+      </c>
+      <c r="B9" s="7">
+        <v>145</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9">
+        <v>162.29596943809688</v>
+      </c>
+      <c r="F9">
+        <v>69.421891154692503</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
+      <c r="A10" s="7">
+        <v>10</v>
+      </c>
+      <c r="B10" s="7">
+        <v>85</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10">
+        <v>160.39388420675371</v>
+      </c>
+      <c r="F10">
+        <v>8.8965527938430003E-4</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
+      <c r="A11" s="7">
+        <v>12</v>
+      </c>
+      <c r="B11" s="7">
+        <v>85</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11">
+        <v>162.16754539251556</v>
+      </c>
+      <c r="F11">
+        <v>11.601307424285451</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
+      <c r="A12" s="7">
+        <v>13</v>
+      </c>
+      <c r="B12" s="7">
+        <v>120</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12">
+        <v>161.66590458807934</v>
+      </c>
+      <c r="F12">
+        <v>3.4966099123584069</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
+      <c r="A13" s="7">
+        <v>14</v>
+      </c>
+      <c r="B13" s="7">
+        <v>120</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13">
+        <v>161.94140267693186</v>
+      </c>
+      <c r="F13">
+        <v>17.198715402852347</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
+      <c r="A14" s="7">
+        <v>15</v>
+      </c>
+      <c r="B14" s="7">
+        <v>120</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14">
+        <v>162.80112356445107</v>
+      </c>
+      <c r="F14">
+        <v>14.892530662050966</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
+      <c r="A15" s="7">
+        <v>16</v>
+      </c>
+      <c r="B15" s="7">
+        <v>145</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15">
+        <v>160.75407959775919</v>
+      </c>
+      <c r="F15">
+        <v>8.9214094531340604E-4</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
+      <c r="A16" s="7">
+        <v>17</v>
+      </c>
+      <c r="B16" s="7">
+        <v>145</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16">
+        <v>161.73770048700803</v>
+      </c>
+      <c r="F16">
+        <v>15.862730271587914</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
+      <c r="C17" s="8"/>
       <c r="D17" s="7"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
+      <c r="C18" s="8"/>
       <c r="D18" s="7"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
+      <c r="C19" s="8"/>
       <c r="D19" s="7"/>
     </row>
   </sheetData>
@@ -777,36 +1062,90 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="2"/>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+    <row r="1" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
+      <c r="A2" s="7">
+        <v>5</v>
+      </c>
+      <c r="B2" s="7">
+        <v>120</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2">
+        <v>163.13595123364951</v>
+      </c>
+      <c r="F2">
+        <v>81.773996381057302</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
+      <c r="A3" s="7">
+        <v>11</v>
+      </c>
+      <c r="B3" s="7">
+        <v>85</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3">
+        <v>162.23912776090114</v>
+      </c>
+      <c r="F3">
+        <v>21.636350153652174</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
+      <c r="A4" s="7">
+        <v>18</v>
+      </c>
+      <c r="B4" s="7">
+        <v>145</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4">
+        <v>162.06572573839108</v>
+      </c>
+      <c r="F4">
+        <v>11.623511691296509</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -817,22 +1156,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1A90CAD-67BE-406A-8BD7-81EDC587CCAA}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.7265625" style="1"/>
     <col min="2" max="2" width="40.90625" style="1" customWidth="1"/>
-    <col min="3" max="4" width="8.7265625" style="1"/>
-    <col min="5" max="5" width="9.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="1"/>
+    <col min="3" max="3" width="12.6328125" style="1" customWidth="1"/>
+    <col min="4" max="5" width="8.7265625" style="1"/>
+    <col min="6" max="6" width="9.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -840,28 +1180,67 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B2" s="3"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B3" s="3"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B4" s="3"/>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="1">
+        <v>85</v>
+      </c>
+      <c r="E2" s="1">
+        <v>145</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E4" xr:uid="{E365AB81-AF3B-4DDA-A9DD-340913AC677F}">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F4" xr:uid="{E365AB81-AF3B-4DDA-A9DD-340913AC677F}">
       <formula1>"Process,Mixture"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C4" xr:uid="{BCCA44C2-9EE1-4675-8860-24289757B621}">
+      <formula1>"Numerical, Categorical"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -874,7 +1253,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -893,12 +1272,20 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="2"/>
-      <c r="B2" s="5"/>
+      <c r="A2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="2"/>
-      <c r="B3" s="5"/>
+      <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added auto-model complefixy selection in Data.xlsx
</commit_message>
<xml_diff>
--- a/src/Data.xlsx
+++ b/src/Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marc\Atmonia Dropbox\Marc Francis Hidalgo\Scripts\How to DoE and ML\ML\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mhidalgo\OneDrive\OneDrive - JLR\Projects\ML\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A8D1A9C-8BED-4507-BE5E-3E6B44D78DA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45622436-0725-4292-A473-3E64E6E9881B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{C1646789-F2F7-4596-96D5-A1743CEE8B52}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{C1646789-F2F7-4596-96D5-A1743CEE8B52}"/>
   </bookViews>
   <sheets>
     <sheet name="Train Data" sheetId="4" r:id="rId1"/>
@@ -166,7 +166,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Features</t>
   </si>
@@ -193,6 +193,12 @@
   </si>
   <si>
     <t>version</t>
+  </si>
+  <si>
+    <t>model</t>
+  </si>
+  <si>
+    <t>Linear</t>
   </si>
 </sst>
 </file>
@@ -663,9 +669,9 @@
       <selection activeCell="B5" sqref="A1:F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -673,109 +679,109 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
       <c r="C2" s="8"/>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="8"/>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="8"/>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="8"/>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8"/>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="8"/>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="8"/>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="8"/>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="8"/>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="8"/>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="8"/>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="8"/>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="8"/>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="8"/>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="8"/>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="8"/>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="8"/>
@@ -796,9 +802,9 @@
       <selection activeCell="D9" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -806,19 +812,19 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
@@ -839,17 +845,17 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="1"/>
-    <col min="2" max="2" width="40.90625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6328125" style="1" customWidth="1"/>
-    <col min="4" max="5" width="8.7265625" style="1"/>
-    <col min="6" max="6" width="9.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="8.7109375" style="1"/>
+    <col min="2" max="2" width="40.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" style="1" customWidth="1"/>
+    <col min="4" max="5" width="8.7109375" style="1"/>
+    <col min="6" max="6" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -869,15 +875,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
     </row>
@@ -903,14 +909,14 @@
       <selection activeCell="A2" sqref="A2:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.7265625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="31.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="23" style="4" customWidth="1"/>
-    <col min="3" max="16384" width="8.7265625" style="1"/>
+    <col min="3" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -918,11 +924,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="5"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="5"/>
     </row>
@@ -934,15 +940,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4CED2DB-40A5-4698-97EC-5128A3B9BBDD}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -950,7 +956,20 @@
         <v>0.2</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{CD6CB0B3-A830-453E-942B-64F485FC9E02}">
+      <formula1>"Linear, 2FI, Quadratic"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>